<commit_message>
addition col to reflect KO Bins
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t xml:space="preserve">assetName</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">etymology</t>
   </si>
   <si>
+    <t xml:space="preserve">stateOfMatter</t>
+  </si>
+  <si>
     <t xml:space="preserve">gold</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">The name derives from the Sanskrit jval for "shine", the Teutonic word gulth for "shining metal", and the Anglo-Saxon gold of unknown origin. The symbol Au derives from the Latin aurum, for Aurora, the goddess of dawn. Gold was known and highly valued in prehistoric times.</t>
   </si>
   <si>
+    <t xml:space="preserve">solid</t>
+  </si>
+  <si>
     <t xml:space="preserve">silver</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
     <t xml:space="preserve">The name derives from the Greek argos for "lazy" or "inactive" because it does not combine with other elements. It was discovered in 1894 by the Scottish chemist William Ramsay and the English physicist Robert John Strutt (Lord Rayleigh) in liquefied air. Rayleigh's initial interest derived from a problem posed by the English physicist Henry Cavendish in 1785, i.e., when oxygen and nitrogen were removed from air, there was an unknown residual gas remaining.</t>
   </si>
   <si>
+    <t xml:space="preserve">gas</t>
+  </si>
+  <si>
     <t xml:space="preserve">boron</t>
   </si>
   <si>
@@ -110,6 +119,24 @@
   </si>
   <si>
     <t xml:space="preserve">The name derives from the Arabic buraq for "white". Although its compounds were known for thousands of years, it was not isolated until 1808 by the French chemists Louis-Joseph Gay-Lussac and Louis-Jacques Thenard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mercury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercury is a chemical element with symbol Hg and atomic number 80. Classified as a transition metal, Mercury is a liquid at room temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Xe]6s24f145d10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name derives from the Roman god Mercury, the nimble messenger of the gods, because the ancients used that name for the element known from prehistoric times. The symbol Hg derives from the Greek hydrargyrum for "liquid silver" or "quick silver".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liquid</t>
   </si>
 </sst>
 </file>
@@ -124,6 +151,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,6 +172,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +217,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,114 +251,156 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="98.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.76"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="471.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added column isotope to data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t xml:space="preserve">assetName</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">sub</t>
   </si>
   <si>
+    <t xml:space="preserve">isotope</t>
+  </si>
+  <si>
     <t xml:space="preserve">etymology</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">Au</t>
   </si>
   <si>
+    <t xml:space="preserve">195 Au, 198 Au</t>
+  </si>
+  <si>
     <t xml:space="preserve">The name derives from the Sanskrit jval for "shine", the Teutonic word gulth for "shining metal", and the Anglo-Saxon gold of unknown origin. The symbol Au derives from the Latin aurum, for Aurora, the goddess of dawn. Gold was known and highly valued in prehistoric times.</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t xml:space="preserve">Ag</t>
   </si>
   <si>
+    <t xml:space="preserve">107 Ag, 109 Ag</t>
+  </si>
+  <si>
     <t xml:space="preserve">The name derives from the Anglo-Saxon seofor and siolfur, which is of unknown origin. The symbol Ag derives from the Latin argentum and Sanskrit argunas from "bright". Silver was known in prehistoric times.</t>
   </si>
   <si>
@@ -85,6 +94,9 @@
     <t xml:space="preserve">Pt</t>
   </si>
   <si>
+    <t xml:space="preserve">190 Pt, 192 pt, 194pt, 195 pt, 196 pt, 198 pt</t>
+  </si>
+  <si>
     <t xml:space="preserve">The name derives from the Spanish platina for "silver". In 1735, the Spanish astronomer Antonio de Ulloa found platinum in Peru, South America. In 1741, the English metallurgist Charles Wood found platinum from Colombia, South America. In 1750, the English physician William Brownrigg prepared purified platinum metal.</t>
   </si>
   <si>
@@ -100,6 +112,9 @@
     <t xml:space="preserve">Ar</t>
   </si>
   <si>
+    <t xml:space="preserve">36 Ar, 38 Ar, 40 Ar</t>
+  </si>
+  <si>
     <t xml:space="preserve">The name derives from the Greek argos for "lazy" or "inactive" because it does not combine with other elements. It was discovered in 1894 by the Scottish chemist William Ramsay and the English physicist Robert John Strutt (Lord Rayleigh) in liquefied air. Rayleigh's initial interest derived from a problem posed by the English physicist Henry Cavendish in 1785, i.e., when oxygen and nitrogen were removed from air, there was an unknown residual gas remaining.</t>
   </si>
   <si>
@@ -118,6 +133,9 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
+    <t xml:space="preserve">10 B, 11 B</t>
+  </si>
+  <si>
     <t xml:space="preserve">The name derives from the Arabic buraq for "white". Although its compounds were known for thousands of years, it was not isolated until 1808 by the French chemists Louis-Joseph Gay-Lussac and Louis-Jacques Thenard.</t>
   </si>
   <si>
@@ -131,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">196 Hg, 198 Hg, 199 Hg, 200 Hg, 201 Hg, 202 Hg, 204 Hg</t>
   </si>
   <si>
     <t xml:space="preserve">The name derives from the Roman god Mercury, the nimble messenger of the gods, because the ancients used that name for the element known from prehistoric times. The symbol Hg derives from the Greek hydrargyrum for "liquid silver" or "quick silver".</t>
@@ -251,16 +272,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="98.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="53.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -279,128 +300,149 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a sort_Values to the gen_annex.py file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Au</t>
   </si>
   <si>
-    <t xml:space="preserve">195 Au, 198 Au</t>
+    <t xml:space="preserve">195 Au; 198 Au</t>
   </si>
   <si>
     <t xml:space="preserve">The name derives from the Sanskrit jval for "shine", the Teutonic word gulth for "shining metal", and the Anglo-Saxon gold of unknown origin. The symbol Au derives from the Latin aurum, for Aurora, the goddess of dawn. Gold was known and highly valued in prehistoric times.</t>
@@ -76,12 +76,72 @@
     <t xml:space="preserve">Ag</t>
   </si>
   <si>
-    <t xml:space="preserve">107 Ag, 109 Ag</t>
+    <t xml:space="preserve">107 Ag; 109 Ag</t>
   </si>
   <si>
     <t xml:space="preserve">The name derives from the Anglo-Saxon seofor and siolfur, which is of unknown origin. The symbol Ag derives from the Latin argentum and Sanskrit argunas from "bright". Silver was known in prehistoric times.</t>
   </si>
   <si>
+    <t xml:space="preserve">argon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon is a chemical element with symbol Ar and atomic number 18. Classified as a noble gas, Argon is a gas at room temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Ne]3s23p6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 Ar; 38 Ar; 40 Ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name derives from the Greek argos for "lazy" or "inactive" because it does not combine with other elements. It was discovered in 1894 by the Scottish chemist William Ramsay and the English physicist Robert John Strutt (Lord Rayleigh) in liquefied air. Rayleigh's initial interest derived from a problem posed by the English physicist Henry Cavendish in 1785, i.e., when oxygen and nitrogen were removed from air, there was an unknown residual gas remaining.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boron is a chemical element with symbol B and atomic number 5. Classified as a metalloid, Boron is a solid at room temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He]2s22p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 B; 11 B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name derives from the Arabic buraq for "white". Although its compounds were known for thousands of years, it was not isolated until 1808 by the French chemists Louis-Joseph Gay-Lussac and Louis-Jacques Thenard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mercury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercury is a chemical element with symbol Hg and atomic number 80. Classified as a transition metal, Mercury is a liquid at room temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Xe]6s24f145d10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">196 Hg; 198 Hg; 199 Hg; 200 Hg; 201 Hg; 202 Hg; 204 Hg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name derives from the Roman god Mercury, the nimble messenger of the gods, because the ancients used that name for the element known from prehistoric times. The symbol Hg derives from the Greek hydrargyrum for "liquid silver" or "quick silver".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liquid</t>
+  </si>
+  <si>
     <t xml:space="preserve">platinum</t>
   </si>
   <si>
@@ -94,70 +154,10 @@
     <t xml:space="preserve">Pt</t>
   </si>
   <si>
-    <t xml:space="preserve">190 Pt, 192 pt, 194pt, 195 pt, 196 pt, 198 pt</t>
+    <t xml:space="preserve">190 Pt; 192 pt; 194pt; 195 pt; 196 pt; 198 pt</t>
   </si>
   <si>
     <t xml:space="preserve">The name derives from the Spanish platina for "silver". In 1735, the Spanish astronomer Antonio de Ulloa found platinum in Peru, South America. In 1741, the English metallurgist Charles Wood found platinum from Colombia, South America. In 1750, the English physician William Brownrigg prepared purified platinum metal.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">argon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon is a chemical element with symbol Ar and atomic number 18. Classified as a noble gas, Argon is a gas at room temperature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Ne]3s23p6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36 Ar, 38 Ar, 40 Ar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name derives from the Greek argos for "lazy" or "inactive" because it does not combine with other elements. It was discovered in 1894 by the Scottish chemist William Ramsay and the English physicist Robert John Strutt (Lord Rayleigh) in liquefied air. Rayleigh's initial interest derived from a problem posed by the English physicist Henry Cavendish in 1785, i.e., when oxygen and nitrogen were removed from air, there was an unknown residual gas remaining.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boron is a chemical element with symbol B and atomic number 5. Classified as a metalloid, Boron is a solid at room temperature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He]2s22p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 B, 11 B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name derives from the Arabic buraq for "white". Although its compounds were known for thousands of years, it was not isolated until 1808 by the French chemists Louis-Joseph Gay-Lussac and Louis-Jacques Thenard.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mercury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercury is a chemical element with symbol Hg and atomic number 80. Classified as a transition metal, Mercury is a liquid at room temperature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Xe]6s24f145d10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">196 Hg, 198 Hg, 199 Hg, 200 Hg, 201 Hg, 202 Hg, 204 Hg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name derives from the Roman god Mercury, the nimble messenger of the gods, because the ancients used that name for the element known from prehistoric times. The symbol Hg derives from the Greek hydrargyrum for "liquid silver" or "quick silver".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liquid</t>
   </si>
 </sst>
 </file>
@@ -274,8 +274,8 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,76 +373,76 @@
         <v>25</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="G7" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload of weekend work
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Boron is a chemical element with symbol B and atomic number 5. Classified as a metalloid, Boron is a solid at room temperature.</t>
   </si>
   <si>
-    <t xml:space="preserve">He]2s22p1</t>
+    <t xml:space="preserve">[He]2s22p1</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -275,10 +275,10 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="53.76"/>

</xml_diff>